<commit_message>
change on db_check finction
</commit_message>
<xml_diff>
--- a/hard-rock.xlsx
+++ b/hard-rock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MT1ShotYT\Desktop\Music-Categorizer\Music-Categorizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666527B7-4B47-45DA-A7A5-DF4355DC1254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CEEF06-28B6-4F8C-8DF3-2C41AA1E7418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3750" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13035" yWindow="5325" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hard-rock" sheetId="1" r:id="rId1"/>
@@ -1894,8 +1894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126"/>
+    <sheetView tabSelected="1" topLeftCell="A270" workbookViewId="0">
+      <selection activeCell="A281" sqref="A281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>